<commit_message>
røret er vendt og data er gemt
</commit_message>
<xml_diff>
--- a/Første lov/førstelovdata.xlsx
+++ b/Første lov/førstelovdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3b4cf22aa3470f28/Documents/GitHub/termo-lab/Første lov/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{496E0959-0307-403A-812E-21BD0280337E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="108" documentId="8_{496E0959-0307-403A-812E-21BD0280337E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6DF03D49-ACF9-4F07-8DEB-BC1C350FBC18}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{AF889908-DF98-4C53-9886-9D1714580EB9}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="9780" windowHeight="11370" activeTab="1" xr2:uid="{AF889908-DF98-4C53-9886-9D1714580EB9}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Forsøg 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Forsøg 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,15 +37,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
     <t>M</t>
   </si>
   <si>
-    <t>T_start</t>
+    <t>T_start [C]</t>
   </si>
   <si>
-    <t>T_slut</t>
+    <t>T_slut [C]</t>
+  </si>
+  <si>
+    <t>Delta_T [K]</t>
   </si>
 </sst>
 </file>
@@ -416,15 +420,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C83862E0-64D3-4471-A13C-EB767B354E79}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,6 +437,396 @@
       </c>
       <c r="C1" t="s">
         <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>26.9</v>
+      </c>
+      <c r="C2">
+        <v>28</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>1.1000000000000014</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>28.3</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D20" si="0">C3-B3</f>
+        <v>0.69999999999999929</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>28.4</v>
+      </c>
+      <c r="C4">
+        <v>29.6</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.2000000000000028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>50</v>
+      </c>
+      <c r="B5">
+        <v>28.5</v>
+      </c>
+      <c r="C5">
+        <v>29.2</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999929</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>52</v>
+      </c>
+      <c r="B6">
+        <v>28.7</v>
+      </c>
+      <c r="C6">
+        <v>29.2</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>50</v>
+      </c>
+      <c r="B7">
+        <v>26.5</v>
+      </c>
+      <c r="C7">
+        <v>27.6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000014</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8">
+        <v>25.6</v>
+      </c>
+      <c r="C8">
+        <v>26.9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>1.2999999999999972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.35">
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56967008-FF33-4A15-B1C2-8F33C322BF69}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2">
+        <v>25.2</v>
+      </c>
+      <c r="C2">
+        <v>28.4</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>3.1999999999999993</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>25.7</v>
+      </c>
+      <c r="C3">
+        <v>28.4</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D13" si="0">C3-B3</f>
+        <v>2.6999999999999993</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>100</v>
+      </c>
+      <c r="B4">
+        <v>25.7</v>
+      </c>
+      <c r="C4">
+        <v>28.2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>150</v>
+      </c>
+      <c r="B5">
+        <v>25.7</v>
+      </c>
+      <c r="C5">
+        <v>29.4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>3.6999999999999993</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <v>25.2</v>
+      </c>
+      <c r="C6">
+        <v>29.4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>4.1999999999999993</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>150</v>
+      </c>
+      <c r="B7">
+        <v>25.2</v>
+      </c>
+      <c r="C7">
+        <v>29.2</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>50</v>
+      </c>
+      <c r="B8">
+        <v>24.7</v>
+      </c>
+      <c r="C8">
+        <v>26.7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>50</v>
+      </c>
+      <c r="B9">
+        <v>25.2</v>
+      </c>
+      <c r="C9">
+        <v>26.8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.6000000000000014</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>50</v>
+      </c>
+      <c r="B10">
+        <v>25.2</v>
+      </c>
+      <c r="C10">
+        <v>26.3</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1.1000000000000014</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>25</v>
+      </c>
+      <c r="C11">
+        <v>25.4</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0.39999999999999858</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>20</v>
+      </c>
+      <c r="B12">
+        <v>25.2</v>
+      </c>
+      <c r="C12">
+        <v>25.9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.69999999999999929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>25.4</v>
+      </c>
+      <c r="C13">
+        <v>25.9</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>